<commit_message>
Actualización de items de gestión
</commit_message>
<xml_diff>
--- a/Desarrollo/BF/Gestión/BF-CP.xlsx
+++ b/Desarrollo/BF/Gestión/BF-CP.xlsx
@@ -8,15 +8,15 @@
     <sheet state="hidden" name="Ideas de proyecto" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_750D806C_93F1_4286_B04D_3841A1501A9B_.wvu.FilterData">Cronograma!$B$9:$I$64</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_57571729_D998_47FF_84A4_37DFE00020E3_.wvu.FilterData">Cronograma!$B$9:$I$64</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_F0AA34F2_93DB_4A4E_BE8C_57081FF25F1F_.wvu.FilterData">Cronograma!$B$9:$I$16</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_929D9260_C6C1_4E11_BE39_CF09C7707A86_.wvu.FilterData">Cronograma!$B$9:$I$64</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_FB89F8EA_A7D9_40AA_B384_5355609E7DC6_.wvu.FilterData">Cronograma!$B$9:$I$64</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_B420B8FC_2E4D_450B_BFFC_2377A9C17799_.wvu.FilterData">Cronograma!$B$9:$I$16</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{F0AA34F2-93DB-4A4E-BE8C-57081FF25F1F}" name="Filtro 1"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{57571729-D998-47FF-84A4-37DFE00020E3}" name="Filtro 2"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{750D806C-93F1-4286-B04D-3841A1501A9B}" name="Filtro 3"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{B420B8FC-2E4D-450B-BFFC-2377A9C17799}" name="Filtro 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{FB89F8EA-A7D9-40AA-B384-5355609E7DC6}" name="Filtro 2"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{929D9260-C6C1-4E11-BE39-CF09C7707A86}" name="Filtro 3"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -1687,10 +1687,10 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="18" fillId="4" fontId="20" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="18" fillId="4" fontId="20" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf borderId="12" fillId="5" fontId="19" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="15" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1734,7 +1734,7 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="27" fillId="2" fontId="17" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="28" fillId="2" fontId="22" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
@@ -2771,8 +2771,8 @@
       <c r="G28" s="46">
         <v>45431.0</v>
       </c>
-      <c r="H28" s="30">
-        <v>0.0</v>
+      <c r="H28" s="41">
+        <v>1.0</v>
       </c>
       <c r="I28" s="30" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H28, {""charttype"", ""bar""; ""max"", 100%})
@@ -2832,7 +2832,7 @@
       </c>
       <c r="H30" s="53">
         <f>AVERAGE(H10:H29)</f>
-        <v>0.905</v>
+        <v>0.955</v>
       </c>
       <c r="I30" s="53" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H30, {""charttype"", ""bar""; ""max"", 100%})
@@ -2865,9 +2865,9 @@
         <v>45435.0</v>
       </c>
       <c r="H31" s="56">
-        <v>0.0</v>
-      </c>
-      <c r="I31" s="56" t="str">
+        <v>1.0</v>
+      </c>
+      <c r="I31" s="57" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H31, {""charttype"", ""bar""; ""max"", 100%})
 "),"")</f>
         <v/>
@@ -2895,9 +2895,9 @@
         <v>45435.0</v>
       </c>
       <c r="H32" s="56">
-        <v>0.0</v>
-      </c>
-      <c r="I32" s="56" t="str">
+        <v>1.0</v>
+      </c>
+      <c r="I32" s="57" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H32, {""charttype"", ""bar""; ""max"", 100%})
 "),"")</f>
         <v/>
@@ -2924,9 +2924,9 @@
         <v>45435.0</v>
       </c>
       <c r="H33" s="56">
-        <v>0.0</v>
-      </c>
-      <c r="I33" s="56" t="str">
+        <v>1.0</v>
+      </c>
+      <c r="I33" s="57" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H33, {""charttype"", ""bar""; ""max"", 100%})
 "),"")</f>
         <v/>
@@ -2952,10 +2952,10 @@
       <c r="G34" s="46">
         <v>45435.0</v>
       </c>
-      <c r="H34" s="57">
-        <v>0.0</v>
-      </c>
-      <c r="I34" s="56" t="str">
+      <c r="H34" s="56">
+        <v>1.0</v>
+      </c>
+      <c r="I34" s="57" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H34, {""charttype"", ""bar""; ""max"", 100%})
 "),"")</f>
         <v/>
@@ -2982,9 +2982,9 @@
         <v>45435.0</v>
       </c>
       <c r="H35" s="56">
-        <v>0.0</v>
-      </c>
-      <c r="I35" s="56" t="str">
+        <v>1.0</v>
+      </c>
+      <c r="I35" s="57" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H35, {""charttype"", ""bar""; ""max"", 100%})
 "),"")</f>
         <v/>
@@ -3011,9 +3011,9 @@
         <v>45435.0</v>
       </c>
       <c r="H36" s="56">
-        <v>0.0</v>
-      </c>
-      <c r="I36" s="56" t="str">
+        <v>1.0</v>
+      </c>
+      <c r="I36" s="57" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H36, {""charttype"", ""bar""; ""max"", 100%})
 "),"")</f>
         <v/>
@@ -3039,9 +3039,9 @@
         <v>45435.0</v>
       </c>
       <c r="H37" s="56">
-        <v>0.0</v>
-      </c>
-      <c r="I37" s="56" t="str">
+        <v>1.0</v>
+      </c>
+      <c r="I37" s="57" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H37, {""charttype"", ""bar""; ""max"", 100%})
 "),"")</f>
         <v/>
@@ -3068,9 +3068,9 @@
         <v>45435.0</v>
       </c>
       <c r="H38" s="56">
-        <v>0.0</v>
-      </c>
-      <c r="I38" s="56" t="str">
+        <v>1.0</v>
+      </c>
+      <c r="I38" s="57" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H38, {""charttype"", ""bar""; ""max"", 100%})
 "),"")</f>
         <v/>
@@ -3097,9 +3097,9 @@
         <v>45438.0</v>
       </c>
       <c r="H39" s="56">
-        <v>0.0</v>
-      </c>
-      <c r="I39" s="56" t="str">
+        <v>1.0</v>
+      </c>
+      <c r="I39" s="57" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H39, {""charttype"", ""bar""; ""max"", 100%})
 "),"")</f>
         <v/>
@@ -3126,9 +3126,9 @@
         <v>45438.0</v>
       </c>
       <c r="H40" s="56">
-        <v>0.0</v>
-      </c>
-      <c r="I40" s="56" t="str">
+        <v>1.0</v>
+      </c>
+      <c r="I40" s="57" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H40, {""charttype"", ""bar""; ""max"", 100%})
 "),"")</f>
         <v/>
@@ -3155,9 +3155,9 @@
         <v>45439.0</v>
       </c>
       <c r="H41" s="56">
-        <v>0.0</v>
-      </c>
-      <c r="I41" s="56" t="str">
+        <v>1.0</v>
+      </c>
+      <c r="I41" s="57" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H41, {""charttype"", ""bar""; ""max"", 100%})
 "),"")</f>
         <v/>
@@ -3188,9 +3188,9 @@
         <v>45446.0</v>
       </c>
       <c r="H42" s="56">
-        <v>0.0</v>
-      </c>
-      <c r="I42" s="56" t="str">
+        <v>1.0</v>
+      </c>
+      <c r="I42" s="57" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H42, {""charttype"", ""bar""; ""max"", 100%})
 "),"")</f>
         <v/>
@@ -3217,10 +3217,10 @@
       <c r="G43" s="29">
         <v>45446.0</v>
       </c>
-      <c r="H43" s="56">
+      <c r="H43" s="57">
         <v>0.0</v>
       </c>
-      <c r="I43" s="56" t="str">
+      <c r="I43" s="57" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H43, {""charttype"", ""bar""; ""max"", 100%})
 "),"")</f>
         <v/>
@@ -3247,10 +3247,10 @@
       <c r="G44" s="29">
         <v>45450.0</v>
       </c>
-      <c r="H44" s="56">
+      <c r="H44" s="57">
         <v>0.0</v>
       </c>
-      <c r="I44" s="56" t="str">
+      <c r="I44" s="57" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H44, {""charttype"", ""bar""; ""max"", 100%})
 "),"")</f>
         <v/>
@@ -3275,7 +3275,7 @@
       </c>
       <c r="H45" s="67">
         <f>AVERAGE(H31:H44)</f>
-        <v>0</v>
+        <v>0.8571428571</v>
       </c>
       <c r="I45" s="67" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H45, {""charttype"", ""bar""; ""max"", 100%})
@@ -3304,8 +3304,8 @@
       <c r="G46" s="29">
         <v>45458.0</v>
       </c>
-      <c r="H46" s="30">
-        <v>0.0</v>
+      <c r="H46" s="41">
+        <v>1.0</v>
       </c>
       <c r="I46" s="30" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H46, {""charttype"", ""bar""; ""max"", 100%})
@@ -3337,8 +3337,8 @@
       <c r="G47" s="29">
         <v>45458.0</v>
       </c>
-      <c r="H47" s="30">
-        <v>0.0</v>
+      <c r="H47" s="41">
+        <v>1.0</v>
       </c>
       <c r="I47" s="30" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H47, {""charttype"", ""bar""; ""max"", 100%})
@@ -3367,8 +3367,8 @@
       <c r="G48" s="29">
         <v>45458.0</v>
       </c>
-      <c r="H48" s="30">
-        <v>0.0</v>
+      <c r="H48" s="41">
+        <v>1.0</v>
       </c>
       <c r="I48" s="30" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H48, {""charttype"", ""bar""; ""max"", 100%})
@@ -3396,8 +3396,8 @@
       <c r="G49" s="29">
         <v>45458.0</v>
       </c>
-      <c r="H49" s="30">
-        <v>0.0</v>
+      <c r="H49" s="41">
+        <v>1.0</v>
       </c>
       <c r="I49" s="30" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H49, {""charttype"", ""bar""; ""max"", 100%})
@@ -3425,8 +3425,8 @@
       <c r="G50" s="29">
         <v>45458.0</v>
       </c>
-      <c r="H50" s="30">
-        <v>0.0</v>
+      <c r="H50" s="41">
+        <v>1.0</v>
       </c>
       <c r="I50" s="30" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H50, {""charttype"", ""bar""; ""max"", 100%})
@@ -3454,8 +3454,8 @@
       <c r="G51" s="29">
         <v>45458.0</v>
       </c>
-      <c r="H51" s="30">
-        <v>0.0</v>
+      <c r="H51" s="41">
+        <v>1.0</v>
       </c>
       <c r="I51" s="30" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H51, {""charttype"", ""bar""; ""max"", 100%})
@@ -3483,8 +3483,8 @@
       <c r="G52" s="29">
         <v>45458.0</v>
       </c>
-      <c r="H52" s="30">
-        <v>0.0</v>
+      <c r="H52" s="41">
+        <v>1.0</v>
       </c>
       <c r="I52" s="30" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H52, {""charttype"", ""bar""; ""max"", 100%})
@@ -3512,8 +3512,8 @@
       <c r="G53" s="29">
         <v>45458.0</v>
       </c>
-      <c r="H53" s="30">
-        <v>0.0</v>
+      <c r="H53" s="41">
+        <v>1.0</v>
       </c>
       <c r="I53" s="30" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H53, {""charttype"", ""bar""; ""max"", 100%})
@@ -3541,8 +3541,8 @@
       <c r="G54" s="29">
         <v>45458.0</v>
       </c>
-      <c r="H54" s="30">
-        <v>0.0</v>
+      <c r="H54" s="41">
+        <v>1.0</v>
       </c>
       <c r="I54" s="30" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H54, {""charttype"", ""bar""; ""max"", 100%})
@@ -3570,8 +3570,8 @@
       <c r="G55" s="29">
         <v>45458.0</v>
       </c>
-      <c r="H55" s="30">
-        <v>0.0</v>
+      <c r="H55" s="41">
+        <v>1.0</v>
       </c>
       <c r="I55" s="30" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H55, {""charttype"", ""bar""; ""max"", 100%})
@@ -3599,8 +3599,8 @@
       <c r="G56" s="29">
         <v>45458.0</v>
       </c>
-      <c r="H56" s="30">
-        <v>0.0</v>
+      <c r="H56" s="41">
+        <v>1.0</v>
       </c>
       <c r="I56" s="30" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H56, {""charttype"", ""bar""; ""max"", 100%})
@@ -3629,11 +3629,11 @@
       <c r="F57" s="28">
         <v>45458.0</v>
       </c>
-      <c r="G57" s="29">
-        <v>45465.0</v>
-      </c>
-      <c r="H57" s="30">
-        <v>0.0</v>
+      <c r="G57" s="46">
+        <v>45466.0</v>
+      </c>
+      <c r="H57" s="41">
+        <v>1.0</v>
       </c>
       <c r="I57" s="30" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H57, {""charttype"", ""bar""; ""max"", 100%})
@@ -3659,11 +3659,11 @@
       <c r="F58" s="28">
         <v>45458.0</v>
       </c>
-      <c r="G58" s="29">
-        <v>45465.0</v>
-      </c>
-      <c r="H58" s="30">
-        <v>0.0</v>
+      <c r="G58" s="46">
+        <v>45466.0</v>
+      </c>
+      <c r="H58" s="41">
+        <v>1.0</v>
       </c>
       <c r="I58" s="30" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H58, {""charttype"", ""bar""; ""max"", 100%})
@@ -3689,8 +3689,8 @@
       <c r="F59" s="28">
         <v>45465.0</v>
       </c>
-      <c r="G59" s="29">
-        <v>45472.0</v>
+      <c r="G59" s="46">
+        <v>45466.0</v>
       </c>
       <c r="H59" s="30">
         <v>0.0</v>
@@ -3719,8 +3719,8 @@
       <c r="F60" s="28">
         <v>45465.0</v>
       </c>
-      <c r="G60" s="29">
-        <v>45472.0</v>
+      <c r="G60" s="46">
+        <v>45466.0</v>
       </c>
       <c r="H60" s="30">
         <v>0.0</v>
@@ -3757,8 +3757,8 @@
       <c r="F61" s="28">
         <v>45465.0</v>
       </c>
-      <c r="G61" s="29">
-        <v>45472.0</v>
+      <c r="G61" s="46">
+        <v>45466.0</v>
       </c>
       <c r="H61" s="30">
         <v>0.0</v>
@@ -3792,11 +3792,11 @@
       <c r="E62" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="F62" s="28">
-        <v>45472.0</v>
-      </c>
-      <c r="G62" s="29">
-        <v>45479.0</v>
+      <c r="F62" s="45">
+        <v>45465.0</v>
+      </c>
+      <c r="G62" s="46">
+        <v>45473.0</v>
       </c>
       <c r="H62" s="30">
         <v>0.0</v>
@@ -3822,11 +3822,11 @@
       <c r="E63" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="F63" s="28">
-        <v>45472.0</v>
-      </c>
-      <c r="G63" s="29">
-        <v>45479.0</v>
+      <c r="F63" s="45">
+        <v>45466.0</v>
+      </c>
+      <c r="G63" s="46">
+        <v>45473.0</v>
       </c>
       <c r="H63" s="30">
         <v>0.0</v>
@@ -3855,11 +3855,11 @@
         <v>45451.0</v>
       </c>
       <c r="G64" s="79">
-        <v>45479.0</v>
+        <v>45473.0</v>
       </c>
       <c r="H64" s="80">
         <f>AVERAGE(H46:H63)</f>
-        <v>0</v>
+        <v>0.7222222222</v>
       </c>
       <c r="I64" s="80" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H64, {""charttype"", ""bar""; ""max"", 100%})
@@ -5784,13 +5784,13 @@
     <row r="1022" ht="15.75" customHeight="1"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{750D806C-93F1-4286-B04D-3841A1501A9B}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{929D9260-C6C1-4E11-BE39-CF09C7707A86}" filter="1" showAutoFilter="1">
       <autoFilter ref="$B$9:$I$64"/>
     </customSheetView>
-    <customSheetView guid="{F0AA34F2-93DB-4A4E-BE8C-57081FF25F1F}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{B420B8FC-2E4D-450B-BFFC-2377A9C17799}" filter="1" showAutoFilter="1">
       <autoFilter ref="$B$9:$I$16"/>
     </customSheetView>
-    <customSheetView guid="{57571729-D998-47FF-84A4-37DFE00020E3}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{FB89F8EA-A7D9-40AA-B384-5355609E7DC6}" filter="1" showAutoFilter="1">
       <autoFilter ref="$B$9:$I$64">
         <filterColumn colId="1">
           <filters>

</xml_diff>

<commit_message>
Verificación y finalización de documentos (análisis)
</commit_message>
<xml_diff>
--- a/Desarrollo/BF/Gestión/BF-CP.xlsx
+++ b/Desarrollo/BF/Gestión/BF-CP.xlsx
@@ -8,15 +8,15 @@
     <sheet state="hidden" name="Ideas de proyecto" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_929D9260_C6C1_4E11_BE39_CF09C7707A86_.wvu.FilterData">Cronograma!$B$9:$I$64</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_FB89F8EA_A7D9_40AA_B384_5355609E7DC6_.wvu.FilterData">Cronograma!$B$9:$I$64</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_B420B8FC_2E4D_450B_BFFC_2377A9C17799_.wvu.FilterData">Cronograma!$B$9:$I$16</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_E8443753_F2FC_4990_A035_9D86299DF228_.wvu.FilterData">Cronograma!$B$9:$I$64</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_35E16094_53CA_4DC5_89C4_A3FFE3E6B88E_.wvu.FilterData">Cronograma!$B$9:$I$16</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_06D732F8_427B_46BD_8806_0816791D9B99_.wvu.FilterData">Cronograma!$B$9:$I$64</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{B420B8FC-2E4D-450B-BFFC-2377A9C17799}" name="Filtro 1"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{FB89F8EA-A7D9-40AA-B384-5355609E7DC6}" name="Filtro 2"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{929D9260-C6C1-4E11-BE39-CF09C7707A86}" name="Filtro 3"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{35E16094-53CA-4DC5-89C4-A3FFE3E6B88E}" name="Filtro 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{E8443753-F2FC-4990-A035-9D86299DF228}" name="Filtro 2"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{06D732F8-427B-46BD-8806-0816791D9B99}" name="Filtro 3"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -385,7 +385,7 @@
     <t>HU_001 - Modular Información de la Página</t>
   </si>
   <si>
-    <t>Modulo Página Principal</t>
+    <t>Módulo Página Principal</t>
   </si>
   <si>
     <t>Lavaud/DB, Arroyo/DF, Saldaña/DF</t>
@@ -3139,7 +3139,7 @@
       <c r="B41" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="C41" s="42" t="s">
+      <c r="C41" s="40" t="s">
         <v>114</v>
       </c>
       <c r="D41" s="26" t="s">
@@ -3217,8 +3217,8 @@
       <c r="G43" s="29">
         <v>45446.0</v>
       </c>
-      <c r="H43" s="57">
-        <v>0.0</v>
+      <c r="H43" s="56">
+        <v>1.0</v>
       </c>
       <c r="I43" s="57" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H43, {""charttype"", ""bar""; ""max"", 100%})
@@ -3247,8 +3247,8 @@
       <c r="G44" s="29">
         <v>45450.0</v>
       </c>
-      <c r="H44" s="57">
-        <v>0.0</v>
+      <c r="H44" s="56">
+        <v>1.0</v>
       </c>
       <c r="I44" s="57" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H44, {""charttype"", ""bar""; ""max"", 100%})
@@ -3275,7 +3275,7 @@
       </c>
       <c r="H45" s="67">
         <f>AVERAGE(H31:H44)</f>
-        <v>0.8571428571</v>
+        <v>1</v>
       </c>
       <c r="I45" s="67" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H45, {""charttype"", ""bar""; ""max"", 100%})
@@ -3692,8 +3692,8 @@
       <c r="G59" s="46">
         <v>45466.0</v>
       </c>
-      <c r="H59" s="30">
-        <v>0.0</v>
+      <c r="H59" s="41">
+        <v>1.0</v>
       </c>
       <c r="I59" s="30" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H59, {""charttype"", ""bar""; ""max"", 100%})
@@ -3722,8 +3722,8 @@
       <c r="G60" s="46">
         <v>45466.0</v>
       </c>
-      <c r="H60" s="30">
-        <v>0.0</v>
+      <c r="H60" s="41">
+        <v>1.0</v>
       </c>
       <c r="I60" s="30" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H60, {""charttype"", ""bar""; ""max"", 100%})
@@ -3760,8 +3760,8 @@
       <c r="G61" s="46">
         <v>45466.0</v>
       </c>
-      <c r="H61" s="30">
-        <v>0.0</v>
+      <c r="H61" s="41">
+        <v>1.0</v>
       </c>
       <c r="I61" s="30" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H61, {""charttype"", ""bar""; ""max"", 100%})
@@ -3798,8 +3798,8 @@
       <c r="G62" s="46">
         <v>45473.0</v>
       </c>
-      <c r="H62" s="30">
-        <v>0.0</v>
+      <c r="H62" s="41">
+        <v>1.0</v>
       </c>
       <c r="I62" s="30" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H62, {""charttype"", ""bar""; ""max"", 100%})
@@ -3828,8 +3828,8 @@
       <c r="G63" s="46">
         <v>45473.0</v>
       </c>
-      <c r="H63" s="30">
-        <v>0.0</v>
+      <c r="H63" s="41">
+        <v>1.0</v>
       </c>
       <c r="I63" s="30" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H63, {""charttype"", ""bar""; ""max"", 100%})
@@ -3859,7 +3859,7 @@
       </c>
       <c r="H64" s="80">
         <f>AVERAGE(H46:H63)</f>
-        <v>0.7222222222</v>
+        <v>1</v>
       </c>
       <c r="I64" s="80" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("SPARKLINE(H64, {""charttype"", ""bar""; ""max"", 100%})
@@ -5784,13 +5784,13 @@
     <row r="1022" ht="15.75" customHeight="1"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{929D9260-C6C1-4E11-BE39-CF09C7707A86}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{06D732F8-427B-46BD-8806-0816791D9B99}" filter="1" showAutoFilter="1">
       <autoFilter ref="$B$9:$I$64"/>
     </customSheetView>
-    <customSheetView guid="{B420B8FC-2E4D-450B-BFFC-2377A9C17799}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{35E16094-53CA-4DC5-89C4-A3FFE3E6B88E}" filter="1" showAutoFilter="1">
       <autoFilter ref="$B$9:$I$16"/>
     </customSheetView>
-    <customSheetView guid="{FB89F8EA-A7D9-40AA-B384-5355609E7DC6}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{E8443753-F2FC-4990-A035-9D86299DF228}" filter="1" showAutoFilter="1">
       <autoFilter ref="$B$9:$I$64">
         <filterColumn colId="1">
           <filters>
@@ -5803,6 +5803,7 @@
             <filter val="Documento de Especificación de Caso de Uso #8"/>
             <filter val="Documento de Especificación de Caso de Uso #7"/>
             <filter val="Documento de Especificación de Caso de Uso #6"/>
+            <filter val="Módulo Página Principal"/>
           </filters>
         </filterColumn>
       </autoFilter>

</xml_diff>